<commit_message>
funcoes trelicas + Pg + Kg
</commit_message>
<xml_diff>
--- a/entrada.xlsx
+++ b/entrada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Downloads\APS4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\APS4-Transcal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA0D96F-4BC3-49F6-8019-9CC01BDAAB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93066978-8C3A-4A90-B328-1C712CC514BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nos" sheetId="1" r:id="rId1"/>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -542,32 +542,60 @@
       <c r="C2" s="2"/>
       <c r="D2" s="9">
         <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>0</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="B3" s="2">
-        <v>0.4</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>0.3</v>
+        <v>0.192</v>
       </c>
       <c r="B4" s="2">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <v>0.432</v>
+      </c>
+      <c r="B7" s="10">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -576,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,15 +641,15 @@
         <v>2</v>
       </c>
       <c r="C2" s="3">
-        <v>210000000000</v>
+        <v>193140000000</v>
       </c>
       <c r="D2" s="3">
-        <v>2.0000000000000001E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="7">
         <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -629,13 +657,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>210000000000</v>
+        <v>193140000000</v>
       </c>
       <c r="D3" s="3">
-        <v>2.0000000000000001E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -643,16 +671,128 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C6" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
-        <v>210000000000</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2.0000000000000001E-4</v>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5.2499999999999997E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>193140000000</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +806,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,58 +831,82 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>150</v>
+        <v>-1300</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="9">
         <f>COUNT(A2:A1048576)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>-100</v>
+        <v>-1500</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-1300</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1500</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-1300</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-1500</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
@@ -867,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="A5:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,17 +1067,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>

</xml_diff>